<commit_message>
Added basic class for Bluetooth
</commit_message>
<xml_diff>
--- a/Allegati/Formulario Ore.xlsx
+++ b/Allegati/Formulario Ore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\workspace\CPTRoverControl\Allegati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F437CE5C-DAAC-4A8F-959A-6AF3C3811EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75BD8B2-9256-49BD-9A15-F958A39C9D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Al</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>Vacanza</t>
+  </si>
+  <si>
+    <t>Analisi tecnologie per sviluppo mobile
+Creazione mockups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analisi tecnologie per sviluppo mobile
+Sviluppo prototipi con Xamarin e React Native
+Scelta finale tecnologia
+</t>
+  </si>
+  <si>
+    <t>Analisi tecnologia Bluetooth
+Revisione mockups
+Creazione Gantt</t>
+  </si>
+  <si>
+    <t>Requisiti funzionali</t>
   </si>
 </sst>
 </file>
@@ -158,47 +176,47 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -484,399 +502,411 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="10"/>
-    <col min="5" max="5" width="75" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="2" width="13.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="75" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+    <row r="3" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>44802</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <f>A3+6</f>
         <v>44808</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>8</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="E3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <f>B3+1</f>
         <v>44809</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <f>A4+6</f>
         <v>44815</v>
       </c>
-      <c r="C4" s="10">
-        <v>16</v>
-      </c>
-      <c r="D4" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="C4" s="8">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <f t="shared" ref="A5:A27" si="0">B4+1</f>
         <v>44816</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <f t="shared" ref="B5:B27" si="1">A5+6</f>
         <v>44822</v>
       </c>
-      <c r="C5" s="10">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="C5" s="8">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8">
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>44823</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <f t="shared" si="1"/>
         <v>44829</v>
       </c>
-      <c r="C6" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="C6" s="8">
+        <v>16</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>44830</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <f t="shared" si="1"/>
         <v>44836</v>
       </c>
-      <c r="C7" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="C7" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>44837</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <f t="shared" si="1"/>
         <v>44843</v>
       </c>
-      <c r="C8" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="C8" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>44844</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <f t="shared" si="1"/>
         <v>44850</v>
       </c>
-      <c r="C9" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="C9" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>44851</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <f t="shared" si="1"/>
         <v>44857</v>
       </c>
-      <c r="C10" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="C10" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>44858</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <f t="shared" si="1"/>
         <v>44864</v>
       </c>
-      <c r="C11" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="C11" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>44865</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <f t="shared" si="1"/>
         <v>44871</v>
       </c>
-      <c r="C12" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="C12" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>44872</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <f t="shared" si="1"/>
         <v>44878</v>
       </c>
-      <c r="C13" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="C13" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>44879</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <f t="shared" si="1"/>
         <v>44885</v>
       </c>
-      <c r="C14" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="C14" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>44886</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <f t="shared" si="1"/>
         <v>44892</v>
       </c>
-      <c r="C15" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="C15" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>44893</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <f t="shared" si="1"/>
         <v>44899</v>
       </c>
-      <c r="C16" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="C16" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>44900</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <f t="shared" si="1"/>
         <v>44906</v>
       </c>
-      <c r="C17" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="C17" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>44907</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <f t="shared" si="1"/>
         <v>44913</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>0</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+    <row r="19" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>44914</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <f t="shared" si="1"/>
         <v>44920</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>0</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+    <row r="20" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>44921</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <f t="shared" si="1"/>
         <v>44927</v>
       </c>
-      <c r="C20" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="C20" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <f t="shared" si="0"/>
         <v>44928</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <f t="shared" si="1"/>
         <v>44934</v>
       </c>
-      <c r="C21" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="C21" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <f t="shared" si="0"/>
         <v>44935</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <f t="shared" si="1"/>
         <v>44941</v>
       </c>
-      <c r="C22" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="C22" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <f t="shared" si="0"/>
         <v>44942</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <f t="shared" si="1"/>
         <v>44948</v>
       </c>
-      <c r="C23" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="C23" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <f t="shared" si="0"/>
         <v>44949</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <f t="shared" si="1"/>
         <v>44955</v>
       </c>
-      <c r="C24" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="C24" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <f t="shared" si="0"/>
         <v>44956</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <f t="shared" si="1"/>
         <v>44962</v>
       </c>
-      <c r="C25" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="C25" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <f>B25+1</f>
         <v>44963</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <f>A26+6</f>
         <v>44969</v>
       </c>
-      <c r="C26" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="C26" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <f t="shared" si="0"/>
         <v>44970</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="7">
         <f t="shared" si="1"/>
         <v>44976</v>
       </c>
-      <c r="C27" s="10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="8" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="13">
+      <c r="C28" s="10">
         <f>SUM(C3:C27)</f>
         <v>360</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:5" ht="60.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A28:B28"/>

</xml_diff>

<commit_message>
Aggiunta elementi mancanti UI
</commit_message>
<xml_diff>
--- a/Allegati/Formulario Ore.xlsx
+++ b/Allegati/Formulario Ore.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\workspace\CPTRoverControl\Allegati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75BD8B2-9256-49BD-9A15-F958A39C9D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E02E6F-C14B-430A-8FDF-87879F2F674C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Al</t>
   </si>
@@ -67,12 +67,6 @@
   <si>
     <t>Analisi tecnologie per sviluppo mobile
 Creazione mockups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analisi tecnologie per sviluppo mobile
-Sviluppo prototipi con Xamarin e React Native
-Scelta finale tecnologia
-</t>
   </si>
   <si>
     <t>Analisi tecnologia Bluetooth
@@ -80,7 +74,22 @@
 Creazione Gantt</t>
   </si>
   <si>
-    <t>Requisiti funzionali</t>
+    <t>Requisiti funzionali
+Inizio sviluppo interfaccia</t>
+  </si>
+  <si>
+    <t>Sviluppo interfaccia
+Inizio sviluppo comunicazione Bluetooth</t>
+  </si>
+  <si>
+    <t>Sviluppo interfaccia
+Gestione permessi dispositivo per Bluetooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analisi tecnologie per sviluppo mobile
+Sviluppo prototipi con Xamarin e React Native
+Scelta finale tecnologia (Xamarin)
+</t>
   </si>
 </sst>
 </file>
@@ -503,7 +512,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -577,7 +586,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -596,7 +605,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -611,8 +620,11 @@
       <c r="C6" s="8">
         <v>16</v>
       </c>
+      <c r="D6" s="8">
+        <v>16</v>
+      </c>
       <c r="E6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -627,6 +639,12 @@
       <c r="C7" s="8">
         <v>16</v>
       </c>
+      <c r="D7" s="8">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -639,6 +657,9 @@
       </c>
       <c r="C8" s="8">
         <v>16</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +924,10 @@
         <f>SUM(C3:C27)</f>
         <v>360</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="10">
+        <f>SUM(D3:D27)</f>
+        <v>72</v>
+      </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" ht="60.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>